<commit_message>
Using openpyxl to preserve excel formulas
</commit_message>
<xml_diff>
--- a/StockData.xlsx
+++ b/StockData.xlsx
@@ -1,95 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharthachapully/Desktop/Python Projects/Stonks/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E562B91C-4092-3E4D-914C-24A740F862D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="StockData" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StockData" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>Stock Value</t>
-  </si>
-  <si>
-    <t>Investment</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>ORCL</t>
-  </si>
-  <si>
-    <t>PREM.L</t>
-  </si>
-  <si>
-    <t>UKOG.L</t>
-  </si>
-  <si>
-    <t>KOD.L</t>
-  </si>
-  <si>
-    <t>TOM.L</t>
-  </si>
-  <si>
-    <t>VELA.L</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>SomeCalc</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -422,179 +419,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>145.38</v>
-      </c>
-      <c r="C2">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Stock Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Investment</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>SomeCalc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>146.14</v>
+      </c>
+      <c r="C2" t="n">
         <v>1000</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D11" si="0">B2/C2</f>
-        <v>0.14538000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>71.790000000000006</v>
-      </c>
-      <c r="C3">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ORCL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>72.97</v>
+      </c>
+      <c r="C3" t="n">
         <v>1000</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>7.1790000000000007E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="C4">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>197.14</v>
+      </c>
+      <c r="C4" t="n">
         <v>1000</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>3.3500000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.13750000000000001</v>
-      </c>
-      <c r="C5">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>UKOG.L</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1425</v>
+      </c>
+      <c r="C5" t="n">
         <v>1000</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1.3750000000000001E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="C6">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>KOD.L</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="C6" t="n">
         <v>1000</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>2.8299999999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="C7">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TOM.L</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="C7" t="n">
         <v>1000</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>4.55E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>3.2500000000000001E-2</v>
-      </c>
-      <c r="C8">
+        <f>B7/C7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>268.75</v>
+      </c>
+      <c r="C8" t="n">
         <v>1000</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>3.2500000000000004E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>270.02</v>
-      </c>
-      <c r="C9">
+        <f>B8/C8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>124.79</v>
+      </c>
+      <c r="C9" t="n">
         <v>1000</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.27001999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>2447</v>
-      </c>
-      <c r="C10">
+        <f>B9/C9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2340.21</v>
+      </c>
+      <c r="C10" t="n">
         <v>1000</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>2.4470000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>2291.2800000000002</v>
-      </c>
-      <c r="C11">
+        <f>B10/C10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>194.25</v>
+      </c>
+      <c r="C11" t="n">
         <v>1000</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>2.29128</v>
-      </c>
-    </row>
+        <f>B11/C11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added scheduling and custom interval in config file
</commit_message>
<xml_diff>
--- a/StockData.xlsx
+++ b/StockData.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>146.14</v>
+        <v>147.96</v>
       </c>
       <c r="C2" t="n">
         <v>1000</v>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72.97</v>
+        <v>71.38</v>
       </c>
       <c r="C3" t="n">
         <v>1000</v>
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>197.14</v>
+        <v>202.83</v>
       </c>
       <c r="C4" t="n">
         <v>1000</v>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1425</v>
+        <v>0.1475</v>
       </c>
       <c r="C5" t="n">
         <v>1000</v>
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.275</v>
+        <v>0.285</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.44</v>
+        <v>0.425</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>268.75</v>
+        <v>270.41</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>124.79</v>
+        <v>121.18</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2340.21</v>
+        <v>2344.76</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>194.25</v>
+        <v>196.64</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>

</xml_diff>